<commit_message>
add export_pembiayaan_screen.dart and function
</commit_message>
<xml_diff>
--- a/assets/form_penilaian_pembiayaan.xlsx
+++ b/assets/form_penilaian_pembiayaan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\githubdownload\flutter_application_1\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07CDBDB3-5548-4D95-ACCF-696C8415CF45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0217C3FA-FDBE-43A7-9090-7E68CB17BDE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{FD05E6C4-AD2B-9C40-9DEB-3E4631342333}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="40">
   <si>
     <t>Header1</t>
   </si>
@@ -616,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3E9FC4D-8050-6F44-B522-43B0D83BF861}">
-  <dimension ref="A1:F13"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -627,7 +627,7 @@
     <col min="4" max="4" width="38.296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -644,7 +644,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="96.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="96.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -660,11 +660,8 @@
       <c r="E2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="165.6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" ht="165.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -681,7 +678,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="132" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -698,7 +695,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="132" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -715,7 +712,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="132" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="132" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -732,7 +729,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -749,7 +746,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -766,7 +763,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="79.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -783,7 +780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="93.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" ht="93.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -800,7 +797,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="124.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" ht="124.8" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -817,7 +814,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="78" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" ht="78" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -834,7 +831,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" ht="62.4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>12</v>
       </c>

</xml_diff>